<commit_message>
feat: criado D_Calendario e medidas
</commit_message>
<xml_diff>
--- a/01 - Supermercado/Data/VENDAS.xlsx
+++ b/01 - Supermercado/Data/VENDAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Neves\Documents\GitHub\PowerBI-Brasil\01 - Supermercado\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D690B5-27A8-4F4D-8B42-DE87B5999388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4842CBF1-7D7A-406F-B985-BFAC8975D1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8015" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8015" uniqueCount="1126">
   <si>
     <t>Invoice ID</t>
   </si>
@@ -3415,6 +3415,15 @@
   </si>
   <si>
     <t>849-09-3807</t>
+  </si>
+  <si>
+    <t>4/25/2019</t>
+  </si>
+  <si>
+    <t>5/4/2019</t>
+  </si>
+  <si>
+    <t>9/4/2019</t>
   </si>
 </sst>
 </file>
@@ -3457,20 +3466,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3545,9 +3554,9 @@
     <tableColumn id="8" xr3:uid="{66F1DA46-2BE9-4A56-B1B8-CF6DD65D1638}" uniqueName="8" name="Quantity" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{01A07BA3-47D3-4A08-BA7B-B26E387F0EFB}" uniqueName="9" name="Tax 5%" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{12518616-E155-45E1-9B76-0A73CA8E8739}" uniqueName="10" name="Total" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{8E2025BC-CC31-47C2-98F2-69EEA6EB7C4D}" uniqueName="11" name="Date" queryTableFieldId="11" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{8E2025BC-CC31-47C2-98F2-69EEA6EB7C4D}" uniqueName="11" name="Date" queryTableFieldId="11" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{52B25AD8-59CD-46CE-B98F-13AD910628E2}" uniqueName="12" name="Time" queryTableFieldId="12" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{407577F1-AE18-4C70-8AE9-949F5B5CEFA0}" uniqueName="13" name="Payment" queryTableFieldId="13" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{407577F1-AE18-4C70-8AE9-949F5B5CEFA0}" uniqueName="13" name="Payment" queryTableFieldId="13" dataDxfId="2"/>
     <tableColumn id="14" xr3:uid="{9537D859-1543-4968-A8DD-27E10FC190A9}" uniqueName="14" name="cogs" queryTableFieldId="14"/>
     <tableColumn id="17" xr3:uid="{5D048306-73E5-400A-90C8-57E9871A7A33}" uniqueName="17" name="Rating" queryTableFieldId="17"/>
   </tableColumns>
@@ -3821,7 +3830,7 @@
   <dimension ref="A1:O1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H1001"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3836,7 +3845,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
@@ -5296,7 +5305,7 @@
         <v>222667.2</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>88</v>
+        <v>1123</v>
       </c>
       <c r="L30" s="2">
         <v>0.82499999999999996</v>
@@ -7452,7 +7461,7 @@
         <v>71324.399999999994</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>75</v>
+        <v>1124</v>
       </c>
       <c r="L74" s="2">
         <v>0.76180555555555551</v>
@@ -10000,7 +10009,7 @@
         <v>83010.899999999994</v>
       </c>
       <c r="K126" s="3" t="s">
-        <v>57</v>
+        <v>1125</v>
       </c>
       <c r="L126" s="2">
         <v>0.62291666666666667</v>

</xml_diff>